<commit_message>
checkpoint grupo 16; feito g13.2
</commit_message>
<xml_diff>
--- a/Data/g13.2.xlsx
+++ b/Data/g13.2.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -392,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>51.28578105476016</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>50.88</v>
       </c>
     </row>
     <row r="3">
@@ -412,11 +488,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>51.13267992212379</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>51.21</v>
       </c>
     </row>
     <row r="4">
@@ -432,11 +508,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>50.48747113657745</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>51.29</v>
       </c>
     </row>
     <row r="5">
@@ -452,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>46.13243293229446</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>51.13</v>
       </c>
     </row>
     <row r="6">
@@ -472,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>46.40541129024624</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>50.49</v>
       </c>
     </row>
     <row r="7">
@@ -492,11 +568,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>48.02080774100882</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>46.13</v>
       </c>
     </row>
     <row r="8">
@@ -512,11 +588,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>48.26400679117148</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>46.41</v>
       </c>
     </row>
     <row r="9">
@@ -532,11 +608,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>49.05990792087598</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>48.02</v>
       </c>
     </row>
     <row r="10">
@@ -552,11 +628,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>50.01221758580504</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>48.26</v>
       </c>
     </row>
     <row r="11">
@@ -572,11 +648,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>50.54599696042929</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>49.06</v>
       </c>
     </row>
     <row r="12">
@@ -592,11 +668,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>50.20649354297969</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>50.01</v>
       </c>
     </row>
     <row r="13">
@@ -612,11 +688,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>50.644573244835</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>50.55</v>
       </c>
     </row>
     <row r="14">
@@ -632,11 +708,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>50.73397663219978</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>50.21</v>
       </c>
     </row>
     <row r="15">
@@ -652,11 +728,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>50.28041736538103</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>50.64</v>
       </c>
     </row>
     <row r="16">
@@ -672,11 +748,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D16">
-        <v>49.8763055346298</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>50.73</v>
       </c>
     </row>
     <row r="17">
@@ -692,11 +768,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D17">
-        <v>49.93175740919557</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>50.28</v>
       </c>
     </row>
     <row r="18">
@@ -712,11 +788,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D18">
-        <v>50.12536671502129</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>49.88</v>
       </c>
     </row>
     <row r="19">
@@ -732,11 +808,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D19">
-        <v>50.46478162897979</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>49.93</v>
       </c>
     </row>
     <row r="20">
@@ -752,11 +828,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D20">
-        <v>50.2716236441915</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>50.13</v>
       </c>
     </row>
     <row r="21">
@@ -772,11 +848,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D21">
-        <v>50.4425227718206</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>50.46</v>
       </c>
     </row>
     <row r="22">
@@ -792,17 +868,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D22">
-        <v>50.66514405698735</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>50.27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -812,17 +888,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D23">
-        <v>44.27124475573578</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>50.44</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -832,11 +908,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D24">
-        <v>44.20076434907612</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>50.67</v>
       </c>
     </row>
     <row r="25">
@@ -852,11 +928,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D25">
-        <v>43.72505077386371</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>43.97</v>
       </c>
     </row>
     <row r="26">
@@ -872,8 +948,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>44.25</v>
       </c>
     </row>
     <row r="27">
@@ -889,8 +968,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>44.27</v>
       </c>
     </row>
     <row r="28">
@@ -906,8 +988,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>44.2</v>
       </c>
     </row>
     <row r="29">
@@ -923,8 +1008,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>43.73</v>
       </c>
     </row>
     <row r="30">
@@ -940,8 +1028,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -957,8 +1048,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -974,8 +1068,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -991,8 +1088,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1008,11 +1108,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D34">
-        <v>43.73755734441271</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1028,11 +1128,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D35">
-        <v>43.96375834284331</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1048,11 +1148,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D36">
-        <v>43.55560160958845</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1068,11 +1168,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D37">
-        <v>42.77828569457142</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1088,11 +1188,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D38">
-        <v>42.80053067764779</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>43.74</v>
       </c>
     </row>
     <row r="39">
@@ -1108,11 +1208,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D39">
-        <v>43.46097581963686</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>43.96</v>
       </c>
     </row>
     <row r="40">
@@ -1128,11 +1228,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D40">
-        <v>43.34118375135377</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>43.56</v>
       </c>
     </row>
     <row r="41">
@@ -1148,11 +1248,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D41">
-        <v>43.09459621889864</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>42.78</v>
       </c>
     </row>
     <row r="42">
@@ -1168,11 +1268,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D42">
-        <v>43.2565479151301</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>42.8</v>
       </c>
     </row>
     <row r="43">
@@ -1188,17 +1288,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D43">
-        <v>43.92015762871584</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>43.46</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1208,17 +1308,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D44">
-        <v>47.63146458061712</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>43.34</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1228,17 +1328,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D45">
-        <v>48.78577623590633</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>43.09</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1248,17 +1348,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D46">
-        <v>46.8628299437473</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>43.26</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1268,8 +1368,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>43.92</v>
       </c>
     </row>
     <row r="48">
@@ -1285,8 +1388,11 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>46.4</v>
       </c>
     </row>
     <row r="49">
@@ -1302,8 +1408,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>47.95</v>
       </c>
     </row>
     <row r="50">
@@ -1319,8 +1428,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>47.63</v>
       </c>
     </row>
     <row r="51">
@@ -1336,8 +1448,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>48.79</v>
       </c>
     </row>
     <row r="52">
@@ -1353,8 +1468,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>46.86</v>
       </c>
     </row>
     <row r="53">
@@ -1370,8 +1488,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1387,8 +1508,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1404,11 +1528,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>46.62420382165605</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1424,11 +1548,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D56">
-        <v>45.76271186440678</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1444,11 +1568,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D57">
-        <v>46.36209813874789</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1464,11 +1588,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D58">
-        <v>44.61798227100042</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1484,11 +1608,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D59">
-        <v>44.43976411120472</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1504,11 +1628,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D60">
-        <v>45.50042052144659</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1524,11 +1648,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D61">
-        <v>44.94334872010072</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>46.62</v>
       </c>
     </row>
     <row r="62">
@@ -1544,11 +1668,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D62">
-        <v>46.585672392124</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>45.76</v>
       </c>
     </row>
     <row r="63">
@@ -1564,11 +1688,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D63">
-        <v>46.69732441471572</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>46.36</v>
       </c>
     </row>
     <row r="64">
@@ -1584,14 +1708,134 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>44.62</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>44.44</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>44.94</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>46.59</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>46.7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D64">
-        <v>46.78631051752922</v>
+      <c r="D70" t="n">
+        <v>46.79</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>